<commit_message>
Keep resolved physio_dashboard.html after merge conflict
</commit_message>
<xml_diff>
--- a/app/docs/admin_features.xlsx
+++ b/app/docs/admin_features.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinap\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinap\Desktop\Agile\Group project\CITS5505-Group-project-Group15\app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F39C87-E079-4E63-9149-607A661B1062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7C579E-E8DA-4F5E-9930-E88B1BDD756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>個人資訊</t>
-  </si>
-  <si>
     <t>姓名、Email、職稱等基本欄位</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
   </si>
   <si>
     <t>&lt;div&gt; 包含 &lt;h3&gt; + 多個 &lt;p&gt;</t>
-  </si>
-  <si>
-    <t>使用者清單總覽</t>
   </si>
   <si>
     <t>表格</t>
@@ -153,6 +147,14 @@
   </si>
   <si>
     <t>Update Log(Manual update)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>個人資訊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用者清單總覽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +505,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -537,16 +539,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -554,67 +556,67 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -622,16 +624,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -639,16 +641,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -656,16 +658,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -673,16 +675,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>